<commit_message>
EPBDS-3786 Update test for case when 0.70*0.75 must be rounded to 0.53 instead of 0.52
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/Round.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/Round.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="round(DoubleValue)" sheetId="1" r:id="rId1"/>
     <sheet name="round(DoubleValue, int)" sheetId="2" r:id="rId2"/>
     <sheet name="round(DoubleValue, int, int)" sheetId="3" r:id="rId3"/>
+    <sheet name="EPBDS-3786" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="196">
   <si>
     <t>Rate</t>
   </si>
@@ -541,6 +542,69 @@
   </si>
   <si>
     <t>-1</t>
+  </si>
+  <si>
+    <t>return round(v1 * v2 ,2);</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>Value 1</t>
+  </si>
+  <si>
+    <t>Value 2</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0.6565</t>
+  </si>
+  <si>
+    <t>0.545454</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>-4.65464</t>
+  </si>
+  <si>
+    <t>-45678.65464</t>
+  </si>
+  <si>
+    <t>212617.69</t>
+  </si>
+  <si>
+    <t>0.55454</t>
+  </si>
+  <si>
+    <t>-89898.8878</t>
+  </si>
+  <si>
+    <t>-49852.53</t>
+  </si>
+  <si>
+    <t>Method double EPBDS3786(double v1, double v2)</t>
+  </si>
+  <si>
+    <t>Test EPBDS3786 EPBDS3786Test</t>
   </si>
 </sst>
 </file>
@@ -592,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -613,12 +677,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y24" sqref="Y24:AA25"/>
     </sheetView>
   </sheetViews>
@@ -946,30 +1014,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="13"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="U5" s="12"/>
+      <c r="U5" s="13"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="12" t="s">
+      <c r="Y5" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="Z5" s="12"/>
+      <c r="Z5" s="13"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -1066,31 +1134,31 @@
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="J11" s="12" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="O11" s="12" t="s">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="O11" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="T11" s="12" t="s">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="T11" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="Y11" s="12" t="s">
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="Y11" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -1707,7 +1775,7 @@
       <c r="E25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -1716,7 +1784,7 @@
       <c r="J25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="L25" s="6" t="s">
@@ -1725,7 +1793,7 @@
       <c r="O25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="Q25" s="6" t="s">
@@ -1734,7 +1802,7 @@
       <c r="T25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="U25" s="13" t="s">
+      <c r="U25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="V25" s="6" t="s">
@@ -1743,7 +1811,7 @@
       <c r="Y25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="Z25" s="13" t="s">
+      <c r="Z25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="AA25" s="6" t="s">
@@ -1771,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:AA80"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="P25" workbookViewId="0">
       <selection activeCell="A81" sqref="A81:XFD99"/>
     </sheetView>
   </sheetViews>
@@ -1795,30 +1863,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="13"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="U5" s="12"/>
+      <c r="U5" s="13"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="12" t="s">
+      <c r="Y5" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="Z5" s="12"/>
+      <c r="Z5" s="13"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -1904,31 +1972,31 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="J11" s="12" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="O11" s="12" t="s">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="O11" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="T11" s="12" t="s">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="T11" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="Y11" s="12" t="s">
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="Y11" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -2529,30 +2597,30 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="4"/>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="4"/>
-      <c r="O30" s="12" t="s">
+      <c r="O30" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="P30" s="12"/>
+      <c r="P30" s="13"/>
       <c r="Q30" s="4"/>
-      <c r="T30" s="12" t="s">
+      <c r="T30" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="U30" s="12"/>
+      <c r="U30" s="13"/>
       <c r="V30" s="4"/>
-      <c r="Y30" s="12" t="s">
+      <c r="Y30" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="Z30" s="12"/>
+      <c r="Z30" s="13"/>
       <c r="AA30" s="4"/>
     </row>
     <row r="31" spans="5:27" x14ac:dyDescent="0.25">
@@ -2638,31 +2706,31 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="J36" s="12" t="s">
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="J36" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="O36" s="12" t="s">
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="O36" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="T36" s="12" t="s">
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="T36" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="Y36" s="12" t="s">
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="Y36" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="12"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
     </row>
     <row r="37" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
@@ -3255,30 +3323,30 @@
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F55" s="12"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="4"/>
-      <c r="J55" s="12" t="s">
+      <c r="J55" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="K55" s="12"/>
+      <c r="K55" s="13"/>
       <c r="L55" s="4"/>
-      <c r="O55" s="12" t="s">
+      <c r="O55" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="P55" s="12"/>
+      <c r="P55" s="13"/>
       <c r="Q55" s="4"/>
-      <c r="T55" s="12" t="s">
+      <c r="T55" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="U55" s="12"/>
+      <c r="U55" s="13"/>
       <c r="V55" s="4"/>
-      <c r="Y55" s="12" t="s">
+      <c r="Y55" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="Z55" s="12"/>
+      <c r="Z55" s="13"/>
       <c r="AA55" s="4"/>
     </row>
     <row r="56" spans="5:27" x14ac:dyDescent="0.25">
@@ -3364,31 +3432,31 @@
       <c r="L60" s="9"/>
     </row>
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="J61" s="12" t="s">
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="J61" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
-      <c r="O61" s="12" t="s">
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="O61" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="T61" s="12" t="s">
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="T61" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="U61" s="12"/>
-      <c r="V61" s="12"/>
-      <c r="Y61" s="12" t="s">
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
+      <c r="Y61" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Z61" s="12"/>
-      <c r="AA61" s="12"/>
+      <c r="Z61" s="13"/>
+      <c r="AA61" s="13"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
@@ -4042,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:AA192"/>
   <sheetViews>
-    <sheetView topLeftCell="R184" workbookViewId="0">
-      <selection activeCell="Y200" sqref="Y200"/>
+    <sheetView topLeftCell="R145" workbookViewId="0">
+      <selection activeCell="T160" sqref="T160:V172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,30 +4134,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="13"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="U5" s="12"/>
+      <c r="U5" s="13"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="12" t="s">
+      <c r="Y5" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="Z5" s="12"/>
+      <c r="Z5" s="13"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -4167,31 +4235,31 @@
       </c>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="J11" s="12" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="O11" s="12" t="s">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="O11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="T11" s="12" t="s">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="T11" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="Y11" s="12" t="s">
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="Y11" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -4758,30 +4826,30 @@
       </c>
     </row>
     <row r="30" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="4"/>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="4"/>
-      <c r="O30" s="12" t="s">
+      <c r="O30" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="P30" s="12"/>
+      <c r="P30" s="13"/>
       <c r="Q30" s="4"/>
-      <c r="T30" s="12" t="s">
+      <c r="T30" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="U30" s="12"/>
+      <c r="U30" s="13"/>
       <c r="V30" s="4"/>
-      <c r="Y30" s="12" t="s">
+      <c r="Y30" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="Z30" s="12"/>
+      <c r="Z30" s="13"/>
       <c r="AA30" s="4"/>
     </row>
     <row r="31" spans="5:27" x14ac:dyDescent="0.25">
@@ -4856,31 +4924,31 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="J36" s="12" t="s">
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="J36" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="O36" s="12" t="s">
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="O36" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="T36" s="12" t="s">
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="T36" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="Y36" s="12" t="s">
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="Y36" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="12"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
     </row>
     <row r="37" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
@@ -5447,30 +5515,30 @@
       </c>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="12"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="4"/>
-      <c r="J55" s="12" t="s">
+      <c r="J55" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="K55" s="12"/>
+      <c r="K55" s="13"/>
       <c r="L55" s="4"/>
-      <c r="O55" s="12" t="s">
+      <c r="O55" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="P55" s="12"/>
+      <c r="P55" s="13"/>
       <c r="Q55" s="4"/>
-      <c r="T55" s="12" t="s">
+      <c r="T55" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="U55" s="12"/>
+      <c r="U55" s="13"/>
       <c r="V55" s="4"/>
-      <c r="Y55" s="12" t="s">
+      <c r="Y55" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="Z55" s="12"/>
+      <c r="Z55" s="13"/>
       <c r="AA55" s="4"/>
     </row>
     <row r="56" spans="5:27" x14ac:dyDescent="0.25">
@@ -5545,31 +5613,31 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="J61" s="12" t="s">
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="J61" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
-      <c r="O61" s="12" t="s">
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="O61" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="T61" s="12" t="s">
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="T61" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="U61" s="12"/>
-      <c r="V61" s="12"/>
-      <c r="Y61" s="12" t="s">
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
+      <c r="Y61" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="Z61" s="12"/>
-      <c r="AA61" s="12"/>
+      <c r="Z61" s="13"/>
+      <c r="AA61" s="13"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
@@ -6136,30 +6204,30 @@
       </c>
     </row>
     <row r="80" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E80" s="12" t="s">
+      <c r="E80" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F80" s="12"/>
+      <c r="F80" s="13"/>
       <c r="G80" s="4"/>
-      <c r="J80" s="12" t="s">
+      <c r="J80" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K80" s="12"/>
+      <c r="K80" s="13"/>
       <c r="L80" s="4"/>
-      <c r="O80" s="12" t="s">
+      <c r="O80" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="P80" s="12"/>
+      <c r="P80" s="13"/>
       <c r="Q80" s="4"/>
-      <c r="T80" s="12" t="s">
+      <c r="T80" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="U80" s="12"/>
+      <c r="U80" s="13"/>
       <c r="V80" s="4"/>
-      <c r="Y80" s="12" t="s">
+      <c r="Y80" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="Z80" s="12"/>
+      <c r="Z80" s="13"/>
       <c r="AA80" s="4"/>
     </row>
     <row r="81" spans="5:27" x14ac:dyDescent="0.25">
@@ -6234,31 +6302,31 @@
       <c r="G85" s="9"/>
     </row>
     <row r="86" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E86" s="12" t="s">
+      <c r="E86" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="J86" s="12" t="s">
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="J86" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="K86" s="12"/>
-      <c r="L86" s="12"/>
-      <c r="O86" s="12" t="s">
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="O86" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="P86" s="12"/>
-      <c r="Q86" s="12"/>
-      <c r="T86" s="12" t="s">
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="T86" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="U86" s="12"/>
-      <c r="V86" s="12"/>
-      <c r="Y86" s="12" t="s">
+      <c r="U86" s="13"/>
+      <c r="V86" s="13"/>
+      <c r="Y86" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="Z86" s="12"/>
-      <c r="AA86" s="12"/>
+      <c r="Z86" s="13"/>
+      <c r="AA86" s="13"/>
     </row>
     <row r="87" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E87" s="10" t="s">
@@ -6825,30 +6893,30 @@
       </c>
     </row>
     <row r="104" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E104" s="12" t="s">
+      <c r="E104" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F104" s="12"/>
+      <c r="F104" s="13"/>
       <c r="G104" s="4"/>
-      <c r="J104" s="12" t="s">
+      <c r="J104" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K104" s="12"/>
+      <c r="K104" s="13"/>
       <c r="L104" s="4"/>
-      <c r="O104" s="12" t="s">
+      <c r="O104" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="P104" s="12"/>
+      <c r="P104" s="13"/>
       <c r="Q104" s="4"/>
-      <c r="T104" s="12" t="s">
+      <c r="T104" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="U104" s="12"/>
+      <c r="U104" s="13"/>
       <c r="V104" s="4"/>
-      <c r="Y104" s="12" t="s">
+      <c r="Y104" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="Z104" s="12"/>
+      <c r="Z104" s="13"/>
       <c r="AA104" s="4"/>
     </row>
     <row r="105" spans="5:27" x14ac:dyDescent="0.25">
@@ -6923,31 +6991,31 @@
       <c r="G109" s="9"/>
     </row>
     <row r="110" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E110" s="12" t="s">
+      <c r="E110" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F110" s="12"/>
-      <c r="G110" s="12"/>
-      <c r="J110" s="12" t="s">
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="J110" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K110" s="12"/>
-      <c r="L110" s="12"/>
-      <c r="O110" s="12" t="s">
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
+      <c r="O110" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="P110" s="12"/>
-      <c r="Q110" s="12"/>
-      <c r="T110" s="12" t="s">
+      <c r="P110" s="13"/>
+      <c r="Q110" s="13"/>
+      <c r="T110" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="U110" s="12"/>
-      <c r="V110" s="12"/>
-      <c r="Y110" s="12" t="s">
+      <c r="U110" s="13"/>
+      <c r="V110" s="13"/>
+      <c r="Y110" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="Z110" s="12"/>
-      <c r="AA110" s="12"/>
+      <c r="Z110" s="13"/>
+      <c r="AA110" s="13"/>
     </row>
     <row r="111" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E111" s="10" t="s">
@@ -7514,30 +7582,30 @@
       </c>
     </row>
     <row r="129" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E129" s="12" t="s">
+      <c r="E129" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F129" s="12"/>
+      <c r="F129" s="13"/>
       <c r="G129" s="4"/>
-      <c r="J129" s="12" t="s">
+      <c r="J129" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K129" s="12"/>
+      <c r="K129" s="13"/>
       <c r="L129" s="4"/>
-      <c r="O129" s="12" t="s">
+      <c r="O129" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="P129" s="12"/>
+      <c r="P129" s="13"/>
       <c r="Q129" s="4"/>
-      <c r="T129" s="12" t="s">
+      <c r="T129" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="U129" s="12"/>
+      <c r="U129" s="13"/>
       <c r="V129" s="4"/>
-      <c r="Y129" s="12" t="s">
+      <c r="Y129" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="Z129" s="12"/>
+      <c r="Z129" s="13"/>
       <c r="AA129" s="4"/>
     </row>
     <row r="130" spans="5:27" x14ac:dyDescent="0.25">
@@ -7612,31 +7680,31 @@
       <c r="G134" s="9"/>
     </row>
     <row r="135" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E135" s="12" t="s">
+      <c r="E135" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F135" s="12"/>
-      <c r="G135" s="12"/>
-      <c r="J135" s="12" t="s">
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="J135" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="K135" s="12"/>
-      <c r="L135" s="12"/>
-      <c r="O135" s="12" t="s">
+      <c r="K135" s="13"/>
+      <c r="L135" s="13"/>
+      <c r="O135" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="P135" s="12"/>
-      <c r="Q135" s="12"/>
-      <c r="T135" s="12" t="s">
+      <c r="P135" s="13"/>
+      <c r="Q135" s="13"/>
+      <c r="T135" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="U135" s="12"/>
-      <c r="V135" s="12"/>
-      <c r="Y135" s="12" t="s">
+      <c r="U135" s="13"/>
+      <c r="V135" s="13"/>
+      <c r="Y135" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="Z135" s="12"/>
-      <c r="AA135" s="12"/>
+      <c r="Z135" s="13"/>
+      <c r="AA135" s="13"/>
     </row>
     <row r="136" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E136" s="10" t="s">
@@ -8203,30 +8271,30 @@
       </c>
     </row>
     <row r="154" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E154" s="12" t="s">
+      <c r="E154" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F154" s="12"/>
+      <c r="F154" s="13"/>
       <c r="G154" s="4"/>
-      <c r="J154" s="12" t="s">
+      <c r="J154" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K154" s="12"/>
+      <c r="K154" s="13"/>
       <c r="L154" s="4"/>
-      <c r="O154" s="12" t="s">
+      <c r="O154" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="P154" s="12"/>
+      <c r="P154" s="13"/>
       <c r="Q154" s="4"/>
-      <c r="T154" s="12" t="s">
+      <c r="T154" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="U154" s="12"/>
+      <c r="U154" s="13"/>
       <c r="V154" s="4"/>
-      <c r="Y154" s="12" t="s">
+      <c r="Y154" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="Z154" s="12"/>
+      <c r="Z154" s="13"/>
       <c r="AA154" s="4"/>
     </row>
     <row r="155" spans="5:27" x14ac:dyDescent="0.25">
@@ -8301,31 +8369,31 @@
       <c r="G159" s="9"/>
     </row>
     <row r="160" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E160" s="12" t="s">
+      <c r="E160" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F160" s="12"/>
-      <c r="G160" s="12"/>
-      <c r="J160" s="12" t="s">
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="J160" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="K160" s="12"/>
-      <c r="L160" s="12"/>
-      <c r="O160" s="12" t="s">
+      <c r="K160" s="13"/>
+      <c r="L160" s="13"/>
+      <c r="O160" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="P160" s="12"/>
-      <c r="Q160" s="12"/>
-      <c r="T160" s="12" t="s">
+      <c r="P160" s="13"/>
+      <c r="Q160" s="13"/>
+      <c r="T160" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="U160" s="12"/>
-      <c r="V160" s="12"/>
-      <c r="Y160" s="12" t="s">
+      <c r="U160" s="13"/>
+      <c r="V160" s="13"/>
+      <c r="Y160" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="Z160" s="12"/>
-      <c r="AA160" s="12"/>
+      <c r="Z160" s="13"/>
+      <c r="AA160" s="13"/>
     </row>
     <row r="161" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E161" s="10" t="s">
@@ -8892,30 +8960,30 @@
       </c>
     </row>
     <row r="179" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E179" s="12" t="s">
+      <c r="E179" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F179" s="12"/>
+      <c r="F179" s="13"/>
       <c r="G179" s="4"/>
-      <c r="J179" s="12" t="s">
+      <c r="J179" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="K179" s="12"/>
+      <c r="K179" s="13"/>
       <c r="L179" s="4"/>
-      <c r="O179" s="12" t="s">
+      <c r="O179" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="P179" s="12"/>
+      <c r="P179" s="13"/>
       <c r="Q179" s="4"/>
-      <c r="T179" s="12" t="s">
+      <c r="T179" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="U179" s="12"/>
+      <c r="U179" s="13"/>
       <c r="V179" s="4"/>
-      <c r="Y179" s="12" t="s">
+      <c r="Y179" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="Z179" s="12"/>
+      <c r="Z179" s="13"/>
       <c r="AA179" s="4"/>
     </row>
     <row r="180" spans="5:27" x14ac:dyDescent="0.25">
@@ -8990,31 +9058,31 @@
       <c r="G184" s="9"/>
     </row>
     <row r="185" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E185" s="12" t="s">
+      <c r="E185" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F185" s="12"/>
-      <c r="G185" s="12"/>
-      <c r="J185" s="12" t="s">
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="J185" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K185" s="12"/>
-      <c r="L185" s="12"/>
-      <c r="O185" s="12" t="s">
+      <c r="K185" s="13"/>
+      <c r="L185" s="13"/>
+      <c r="O185" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="P185" s="12"/>
-      <c r="Q185" s="12"/>
-      <c r="T185" s="12" t="s">
+      <c r="P185" s="13"/>
+      <c r="Q185" s="13"/>
+      <c r="T185" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="U185" s="12"/>
-      <c r="V185" s="12"/>
-      <c r="Y185" s="12" t="s">
+      <c r="U185" s="13"/>
+      <c r="V185" s="13"/>
+      <c r="Y185" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="Z185" s="12"/>
-      <c r="AA185" s="12"/>
+      <c r="Z185" s="13"/>
+      <c r="AA185" s="13"/>
     </row>
     <row r="186" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E186" s="10" t="s">
@@ -9430,4 +9498,136 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3">
+        <v>6565</v>
+      </c>
+      <c r="D16" s="3">
+        <v>433290</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-6542 Add test for 'Method round(java.lang.Integer) is ambiguous'
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/Round.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/Round.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290" activeTab="3"/>
@@ -10,14 +10,14 @@
     <sheet name="round(DoubleValue)" sheetId="1" r:id="rId1"/>
     <sheet name="round(DoubleValue, int)" sheetId="2" r:id="rId2"/>
     <sheet name="round(DoubleValue, int, int)" sheetId="3" r:id="rId3"/>
-    <sheet name="EPBDS-3786" sheetId="4" r:id="rId4"/>
+    <sheet name="EPBDS Issues" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="212">
   <si>
     <t>Rate</t>
   </si>
@@ -605,19 +605,74 @@
   </si>
   <si>
     <t>Test EPBDS3786 EPBDS3786Test</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>case1</t>
+  </si>
+  <si>
+    <t>=int</t>
+  </si>
+  <si>
+    <t>case2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult EPBDS6542(Integer int)</t>
+  </si>
+  <si>
+    <t>case3</t>
+  </si>
+  <si>
+    <t>=round(int)</t>
+  </si>
+  <si>
+    <t>=round($case1)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>case4</t>
+  </si>
+  <si>
+    <t>case5</t>
+  </si>
+  <si>
+    <t>Test EPBDS6542 EPBDS6542Test</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$case2</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$case3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -653,10 +708,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -680,16 +736,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1014,30 +1078,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="K5" s="13"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="P5" s="13"/>
+      <c r="P5" s="15"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="U5" s="13"/>
+      <c r="U5" s="15"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Z5" s="13"/>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -1134,31 +1198,31 @@
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="J11" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="O11" s="13" t="s">
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="O11" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="T11" s="13" t="s">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="T11" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="Y11" s="13" t="s">
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="Y11" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -1863,30 +1927,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="13"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="P5" s="13"/>
+      <c r="P5" s="15"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="U5" s="13"/>
+      <c r="U5" s="15"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="Z5" s="13"/>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -1972,31 +2036,31 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="J11" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="O11" s="13" t="s">
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="O11" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="T11" s="13" t="s">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="T11" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="Y11" s="13" t="s">
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="Y11" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -2597,30 +2661,30 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="13"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="4"/>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="K30" s="13"/>
+      <c r="K30" s="15"/>
       <c r="L30" s="4"/>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="P30" s="13"/>
+      <c r="P30" s="15"/>
       <c r="Q30" s="4"/>
-      <c r="T30" s="13" t="s">
+      <c r="T30" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="U30" s="13"/>
+      <c r="U30" s="15"/>
       <c r="V30" s="4"/>
-      <c r="Y30" s="13" t="s">
+      <c r="Y30" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="Z30" s="13"/>
+      <c r="Z30" s="15"/>
       <c r="AA30" s="4"/>
     </row>
     <row r="31" spans="5:27" x14ac:dyDescent="0.25">
@@ -2706,31 +2770,31 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="J36" s="13" t="s">
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="J36" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="O36" s="13" t="s">
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="O36" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="T36" s="13" t="s">
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="T36" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="Y36" s="13" t="s">
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="Y36" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
     </row>
     <row r="37" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
@@ -3323,30 +3387,30 @@
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F55" s="13"/>
+      <c r="F55" s="15"/>
       <c r="G55" s="4"/>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="K55" s="13"/>
+      <c r="K55" s="15"/>
       <c r="L55" s="4"/>
-      <c r="O55" s="13" t="s">
+      <c r="O55" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="P55" s="13"/>
+      <c r="P55" s="15"/>
       <c r="Q55" s="4"/>
-      <c r="T55" s="13" t="s">
+      <c r="T55" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="U55" s="13"/>
+      <c r="U55" s="15"/>
       <c r="V55" s="4"/>
-      <c r="Y55" s="13" t="s">
+      <c r="Y55" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z55" s="13"/>
+      <c r="Z55" s="15"/>
       <c r="AA55" s="4"/>
     </row>
     <row r="56" spans="5:27" x14ac:dyDescent="0.25">
@@ -3432,31 +3496,31 @@
       <c r="L60" s="9"/>
     </row>
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="J61" s="13" t="s">
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="J61" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="O61" s="13" t="s">
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="O61" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="T61" s="13" t="s">
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="T61" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="U61" s="13"/>
-      <c r="V61" s="13"/>
-      <c r="Y61" s="13" t="s">
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="Y61" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="Z61" s="13"/>
-      <c r="AA61" s="13"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
@@ -4134,30 +4198,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="4"/>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="13"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="P5" s="13"/>
+      <c r="P5" s="15"/>
       <c r="Q5" s="4"/>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="U5" s="13"/>
+      <c r="U5" s="15"/>
       <c r="V5" s="4"/>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="Z5" s="13"/>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="5:27" x14ac:dyDescent="0.25">
@@ -4235,31 +4299,31 @@
       </c>
     </row>
     <row r="11" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="J11" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="O11" s="13" t="s">
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="O11" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="T11" s="13" t="s">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="T11" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="Y11" s="13" t="s">
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="Y11" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
     </row>
     <row r="12" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
@@ -4826,30 +4890,30 @@
       </c>
     </row>
     <row r="30" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="13"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="4"/>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="K30" s="13"/>
+      <c r="K30" s="15"/>
       <c r="L30" s="4"/>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="P30" s="13"/>
+      <c r="P30" s="15"/>
       <c r="Q30" s="4"/>
-      <c r="T30" s="13" t="s">
+      <c r="T30" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="U30" s="13"/>
+      <c r="U30" s="15"/>
       <c r="V30" s="4"/>
-      <c r="Y30" s="13" t="s">
+      <c r="Y30" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="Z30" s="13"/>
+      <c r="Z30" s="15"/>
       <c r="AA30" s="4"/>
     </row>
     <row r="31" spans="5:27" x14ac:dyDescent="0.25">
@@ -4924,31 +4988,31 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="J36" s="13" t="s">
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="J36" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="O36" s="13" t="s">
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="O36" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="T36" s="13" t="s">
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="T36" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="Y36" s="13" t="s">
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="Y36" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
     </row>
     <row r="37" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
@@ -5515,30 +5579,30 @@
       </c>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="13"/>
+      <c r="F55" s="15"/>
       <c r="G55" s="4"/>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="K55" s="13"/>
+      <c r="K55" s="15"/>
       <c r="L55" s="4"/>
-      <c r="O55" s="13" t="s">
+      <c r="O55" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="P55" s="13"/>
+      <c r="P55" s="15"/>
       <c r="Q55" s="4"/>
-      <c r="T55" s="13" t="s">
+      <c r="T55" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="U55" s="13"/>
+      <c r="U55" s="15"/>
       <c r="V55" s="4"/>
-      <c r="Y55" s="13" t="s">
+      <c r="Y55" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="Z55" s="13"/>
+      <c r="Z55" s="15"/>
       <c r="AA55" s="4"/>
     </row>
     <row r="56" spans="5:27" x14ac:dyDescent="0.25">
@@ -5613,31 +5677,31 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="J61" s="13" t="s">
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="J61" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="O61" s="13" t="s">
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="O61" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="T61" s="13" t="s">
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="T61" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="U61" s="13"/>
-      <c r="V61" s="13"/>
-      <c r="Y61" s="13" t="s">
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="Y61" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="Z61" s="13"/>
-      <c r="AA61" s="13"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
@@ -6204,30 +6268,30 @@
       </c>
     </row>
     <row r="80" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E80" s="13" t="s">
+      <c r="E80" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F80" s="13"/>
+      <c r="F80" s="15"/>
       <c r="G80" s="4"/>
-      <c r="J80" s="13" t="s">
+      <c r="J80" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="K80" s="13"/>
+      <c r="K80" s="15"/>
       <c r="L80" s="4"/>
-      <c r="O80" s="13" t="s">
+      <c r="O80" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="P80" s="13"/>
+      <c r="P80" s="15"/>
       <c r="Q80" s="4"/>
-      <c r="T80" s="13" t="s">
+      <c r="T80" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="U80" s="13"/>
+      <c r="U80" s="15"/>
       <c r="V80" s="4"/>
-      <c r="Y80" s="13" t="s">
+      <c r="Y80" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="Z80" s="13"/>
+      <c r="Z80" s="15"/>
       <c r="AA80" s="4"/>
     </row>
     <row r="81" spans="5:27" x14ac:dyDescent="0.25">
@@ -6302,31 +6366,31 @@
       <c r="G85" s="9"/>
     </row>
     <row r="86" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E86" s="13" t="s">
+      <c r="E86" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="J86" s="13" t="s">
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="J86" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="O86" s="13" t="s">
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="O86" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="13"/>
-      <c r="T86" s="13" t="s">
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="T86" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="U86" s="13"/>
-      <c r="V86" s="13"/>
-      <c r="Y86" s="13" t="s">
+      <c r="U86" s="15"/>
+      <c r="V86" s="15"/>
+      <c r="Y86" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="Z86" s="13"/>
-      <c r="AA86" s="13"/>
+      <c r="Z86" s="15"/>
+      <c r="AA86" s="15"/>
     </row>
     <row r="87" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E87" s="10" t="s">
@@ -6893,30 +6957,30 @@
       </c>
     </row>
     <row r="104" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E104" s="13" t="s">
+      <c r="E104" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F104" s="13"/>
+      <c r="F104" s="15"/>
       <c r="G104" s="4"/>
-      <c r="J104" s="13" t="s">
+      <c r="J104" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K104" s="13"/>
+      <c r="K104" s="15"/>
       <c r="L104" s="4"/>
-      <c r="O104" s="13" t="s">
+      <c r="O104" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="P104" s="13"/>
+      <c r="P104" s="15"/>
       <c r="Q104" s="4"/>
-      <c r="T104" s="13" t="s">
+      <c r="T104" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="U104" s="13"/>
+      <c r="U104" s="15"/>
       <c r="V104" s="4"/>
-      <c r="Y104" s="13" t="s">
+      <c r="Y104" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="Z104" s="13"/>
+      <c r="Z104" s="15"/>
       <c r="AA104" s="4"/>
     </row>
     <row r="105" spans="5:27" x14ac:dyDescent="0.25">
@@ -6991,31 +7055,31 @@
       <c r="G109" s="9"/>
     </row>
     <row r="110" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E110" s="13" t="s">
+      <c r="E110" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="J110" s="13" t="s">
+      <c r="F110" s="15"/>
+      <c r="G110" s="15"/>
+      <c r="J110" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="K110" s="13"/>
-      <c r="L110" s="13"/>
-      <c r="O110" s="13" t="s">
+      <c r="K110" s="15"/>
+      <c r="L110" s="15"/>
+      <c r="O110" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="P110" s="13"/>
-      <c r="Q110" s="13"/>
-      <c r="T110" s="13" t="s">
+      <c r="P110" s="15"/>
+      <c r="Q110" s="15"/>
+      <c r="T110" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="U110" s="13"/>
-      <c r="V110" s="13"/>
-      <c r="Y110" s="13" t="s">
+      <c r="U110" s="15"/>
+      <c r="V110" s="15"/>
+      <c r="Y110" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="Z110" s="13"/>
-      <c r="AA110" s="13"/>
+      <c r="Z110" s="15"/>
+      <c r="AA110" s="15"/>
     </row>
     <row r="111" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E111" s="10" t="s">
@@ -7582,30 +7646,30 @@
       </c>
     </row>
     <row r="129" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E129" s="13" t="s">
+      <c r="E129" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F129" s="13"/>
+      <c r="F129" s="15"/>
       <c r="G129" s="4"/>
-      <c r="J129" s="13" t="s">
+      <c r="J129" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="K129" s="13"/>
+      <c r="K129" s="15"/>
       <c r="L129" s="4"/>
-      <c r="O129" s="13" t="s">
+      <c r="O129" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="P129" s="13"/>
+      <c r="P129" s="15"/>
       <c r="Q129" s="4"/>
-      <c r="T129" s="13" t="s">
+      <c r="T129" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="U129" s="13"/>
+      <c r="U129" s="15"/>
       <c r="V129" s="4"/>
-      <c r="Y129" s="13" t="s">
+      <c r="Y129" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="Z129" s="13"/>
+      <c r="Z129" s="15"/>
       <c r="AA129" s="4"/>
     </row>
     <row r="130" spans="5:27" x14ac:dyDescent="0.25">
@@ -7680,31 +7744,31 @@
       <c r="G134" s="9"/>
     </row>
     <row r="135" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E135" s="13" t="s">
+      <c r="E135" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
-      <c r="J135" s="13" t="s">
+      <c r="F135" s="15"/>
+      <c r="G135" s="15"/>
+      <c r="J135" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="K135" s="13"/>
-      <c r="L135" s="13"/>
-      <c r="O135" s="13" t="s">
+      <c r="K135" s="15"/>
+      <c r="L135" s="15"/>
+      <c r="O135" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="P135" s="13"/>
-      <c r="Q135" s="13"/>
-      <c r="T135" s="13" t="s">
+      <c r="P135" s="15"/>
+      <c r="Q135" s="15"/>
+      <c r="T135" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="U135" s="13"/>
-      <c r="V135" s="13"/>
-      <c r="Y135" s="13" t="s">
+      <c r="U135" s="15"/>
+      <c r="V135" s="15"/>
+      <c r="Y135" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="Z135" s="13"/>
-      <c r="AA135" s="13"/>
+      <c r="Z135" s="15"/>
+      <c r="AA135" s="15"/>
     </row>
     <row r="136" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E136" s="10" t="s">
@@ -8271,30 +8335,30 @@
       </c>
     </row>
     <row r="154" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E154" s="13" t="s">
+      <c r="E154" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F154" s="13"/>
+      <c r="F154" s="15"/>
       <c r="G154" s="4"/>
-      <c r="J154" s="13" t="s">
+      <c r="J154" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K154" s="13"/>
+      <c r="K154" s="15"/>
       <c r="L154" s="4"/>
-      <c r="O154" s="13" t="s">
+      <c r="O154" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="P154" s="13"/>
+      <c r="P154" s="15"/>
       <c r="Q154" s="4"/>
-      <c r="T154" s="13" t="s">
+      <c r="T154" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="U154" s="13"/>
+      <c r="U154" s="15"/>
       <c r="V154" s="4"/>
-      <c r="Y154" s="13" t="s">
+      <c r="Y154" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="Z154" s="13"/>
+      <c r="Z154" s="15"/>
       <c r="AA154" s="4"/>
     </row>
     <row r="155" spans="5:27" x14ac:dyDescent="0.25">
@@ -8369,31 +8433,31 @@
       <c r="G159" s="9"/>
     </row>
     <row r="160" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E160" s="13" t="s">
+      <c r="E160" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F160" s="13"/>
-      <c r="G160" s="13"/>
-      <c r="J160" s="13" t="s">
+      <c r="F160" s="15"/>
+      <c r="G160" s="15"/>
+      <c r="J160" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="K160" s="13"/>
-      <c r="L160" s="13"/>
-      <c r="O160" s="13" t="s">
+      <c r="K160" s="15"/>
+      <c r="L160" s="15"/>
+      <c r="O160" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="P160" s="13"/>
-      <c r="Q160" s="13"/>
-      <c r="T160" s="13" t="s">
+      <c r="P160" s="15"/>
+      <c r="Q160" s="15"/>
+      <c r="T160" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="U160" s="13"/>
-      <c r="V160" s="13"/>
-      <c r="Y160" s="13" t="s">
+      <c r="U160" s="15"/>
+      <c r="V160" s="15"/>
+      <c r="Y160" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="Z160" s="13"/>
-      <c r="AA160" s="13"/>
+      <c r="Z160" s="15"/>
+      <c r="AA160" s="15"/>
     </row>
     <row r="161" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E161" s="10" t="s">
@@ -8960,30 +9024,30 @@
       </c>
     </row>
     <row r="179" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E179" s="13" t="s">
+      <c r="E179" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F179" s="13"/>
+      <c r="F179" s="15"/>
       <c r="G179" s="4"/>
-      <c r="J179" s="13" t="s">
+      <c r="J179" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="K179" s="13"/>
+      <c r="K179" s="15"/>
       <c r="L179" s="4"/>
-      <c r="O179" s="13" t="s">
+      <c r="O179" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="P179" s="13"/>
+      <c r="P179" s="15"/>
       <c r="Q179" s="4"/>
-      <c r="T179" s="13" t="s">
+      <c r="T179" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="U179" s="13"/>
+      <c r="U179" s="15"/>
       <c r="V179" s="4"/>
-      <c r="Y179" s="13" t="s">
+      <c r="Y179" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="Z179" s="13"/>
+      <c r="Z179" s="15"/>
       <c r="AA179" s="4"/>
     </row>
     <row r="180" spans="5:27" x14ac:dyDescent="0.25">
@@ -9058,31 +9122,31 @@
       <c r="G184" s="9"/>
     </row>
     <row r="185" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E185" s="13" t="s">
+      <c r="E185" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F185" s="13"/>
-      <c r="G185" s="13"/>
-      <c r="J185" s="13" t="s">
+      <c r="F185" s="15"/>
+      <c r="G185" s="15"/>
+      <c r="J185" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="K185" s="13"/>
-      <c r="L185" s="13"/>
-      <c r="O185" s="13" t="s">
+      <c r="K185" s="15"/>
+      <c r="L185" s="15"/>
+      <c r="O185" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="P185" s="13"/>
-      <c r="Q185" s="13"/>
-      <c r="T185" s="13" t="s">
+      <c r="P185" s="15"/>
+      <c r="Q185" s="15"/>
+      <c r="T185" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="U185" s="13"/>
-      <c r="V185" s="13"/>
-      <c r="Y185" s="13" t="s">
+      <c r="U185" s="15"/>
+      <c r="V185" s="15"/>
+      <c r="Y185" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="Z185" s="13"/>
-      <c r="AA185" s="13"/>
+      <c r="Z185" s="15"/>
+      <c r="AA185" s="15"/>
     </row>
     <row r="186" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E186" s="10" t="s">
@@ -9502,39 +9566,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D16"/>
+  <dimension ref="B4:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="F4" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="F5" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>176</v>
       </c>
@@ -9545,7 +9654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>178</v>
       </c>
@@ -9556,7 +9665,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>184</v>
       </c>
@@ -9566,8 +9675,14 @@
       <c r="D11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -9577,8 +9692,20 @@
       <c r="D12" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>188</v>
       </c>
@@ -9588,8 +9715,20 @@
       <c r="D13" s="3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>181</v>
       </c>
@@ -9599,8 +9738,20 @@
       <c r="D14" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>191</v>
       </c>
@@ -9610,8 +9761,20 @@
       <c r="D15" s="3" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>66</v>
       </c>
@@ -9621,12 +9784,58 @@
       <c r="D16" s="3">
         <v>433290</v>
       </c>
+      <c r="F16" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-1000000000</v>
+      </c>
+      <c r="H18" s="3">
+        <v>-1000000000</v>
+      </c>
+      <c r="I18" s="3">
+        <v>-1000000000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B8:D8"/>
+  <mergeCells count="9">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>